<commit_message>
Sparse Method 1 Complete
</commit_message>
<xml_diff>
--- a/DjikstraComparisons.xlsx
+++ b/DjikstraComparisons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>List</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Number of verticies</t>
-  </si>
-  <si>
-    <t>Types of Graphs (Time to Compute)</t>
   </si>
   <si>
     <t>Sparse Graph Method 1</t>
@@ -50,14 +47,17 @@
     <t>Dense Graph Method 2</t>
   </si>
   <si>
-    <t>Types of Graphs (Time to Compute in seconds)</t>
+    <t>Time to Create Graph (seconds)</t>
+  </si>
+  <si>
+    <t>Time to Run Algorithem (seconds)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +72,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -81,9 +87,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -93,14 +108,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,28 +409,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -412,212 +444,796 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10</v>
       </c>
+      <c r="B3">
+        <v>0.02</v>
+      </c>
       <c r="C3">
+        <v>0.02</v>
+      </c>
+      <c r="D3" s="9">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="10">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>0.02</v>
+      </c>
+      <c r="C4">
+        <v>0.02</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+      <c r="C5">
+        <v>0.02</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>75</v>
+      </c>
+      <c r="B6">
+        <v>0.01</v>
+      </c>
+      <c r="C6">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>100</v>
       </c>
-      <c r="C4">
+      <c r="B7">
+        <v>0.01</v>
+      </c>
+      <c r="C7">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="E7" s="11">
         <v>0.03</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>125</v>
+      </c>
+      <c r="B8">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>150</v>
+      </c>
+      <c r="B9">
+        <v>0.02</v>
+      </c>
+      <c r="C9">
+        <v>0.03</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>175</v>
+      </c>
+      <c r="B10">
+        <v>0.03</v>
+      </c>
+      <c r="C10">
+        <v>0.02</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>200</v>
+      </c>
+      <c r="B11">
+        <v>0.01</v>
+      </c>
+      <c r="C11">
+        <v>0.03</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>250</v>
+      </c>
+      <c r="B12">
+        <v>0.02</v>
+      </c>
+      <c r="C12">
+        <v>0.03</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.11</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>500</v>
+      </c>
+      <c r="B13">
+        <v>0.01</v>
+      </c>
+      <c r="C13">
+        <v>0.02</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.67</v>
+      </c>
+      <c r="E13" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>750</v>
+      </c>
+      <c r="B14">
+        <v>0.02</v>
+      </c>
+      <c r="C14">
+        <v>0.05</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2.27</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>1000</v>
       </c>
-      <c r="C5">
+      <c r="B15">
+        <v>0.02</v>
+      </c>
+      <c r="C15">
+        <v>0.04</v>
+      </c>
+      <c r="D15" s="9">
+        <v>5.86</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1250</v>
+      </c>
+      <c r="B16">
+        <v>0.02</v>
+      </c>
+      <c r="C16">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="9">
+        <v>12.37</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C17">
+        <v>0.11</v>
+      </c>
+      <c r="D17" s="9">
+        <v>22.02</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1750</v>
+      </c>
+      <c r="B18">
+        <v>0.03</v>
+      </c>
+      <c r="C18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D18" s="9">
+        <v>36.19</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B19">
+        <v>0.03</v>
+      </c>
+      <c r="C19">
+        <v>0.08</v>
+      </c>
+      <c r="D19" s="9">
+        <v>55.04</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2500</v>
+      </c>
+      <c r="B20">
+        <v>0.04</v>
+      </c>
+      <c r="C20">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>10000</v>
-      </c>
-      <c r="C6">
-        <v>2.65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>100000</v>
-      </c>
-      <c r="C7">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="C8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="D20" s="9">
+        <v>108.82</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B21">
+        <v>0.06</v>
+      </c>
+      <c r="C21">
+        <v>0.35</v>
+      </c>
+      <c r="D21" s="9">
+        <v>980.61</v>
+      </c>
+      <c r="E21" s="11">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>50</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>75</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>125</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>150</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>175</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>200</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>250</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>500</v>
+      </c>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>750</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>1250</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1750</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>2500</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>10</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>25</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>50</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>75</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>100</v>
+      </c>
+      <c r="D51" s="9"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>125</v>
+      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>150</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>175</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>200</v>
+      </c>
+      <c r="D55" s="9"/>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>250</v>
+      </c>
+      <c r="D56" s="9"/>
+      <c r="E56" s="10"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>500</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>750</v>
+      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D59" s="9"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>1250</v>
+      </c>
+      <c r="D60" s="9"/>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D61" s="9"/>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>1750</v>
+      </c>
+      <c r="D62" s="9"/>
+      <c r="E62" s="10"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D63" s="9"/>
+      <c r="E63" s="10"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>2500</v>
+      </c>
+      <c r="D64" s="9"/>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D65" s="9"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="9"/>
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="10"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="D69" s="9"/>
+      <c r="E69" s="10"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>25</v>
+      </c>
+      <c r="D70" s="9"/>
+      <c r="E70" s="10"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>50</v>
+      </c>
+      <c r="D71" s="9"/>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>75</v>
+      </c>
+      <c r="D72" s="9"/>
+      <c r="E72" s="10"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="D73" s="9"/>
+      <c r="E73" s="10"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>125</v>
+      </c>
+      <c r="D74" s="9"/>
+      <c r="E74" s="10"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>150</v>
+      </c>
+      <c r="D75" s="9"/>
+      <c r="E75" s="10"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>175</v>
+      </c>
+      <c r="D76" s="9"/>
+      <c r="E76" s="10"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>200</v>
+      </c>
+      <c r="D77" s="9"/>
+      <c r="E77" s="10"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>250</v>
+      </c>
+      <c r="D78" s="9"/>
+      <c r="E78" s="10"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>500</v>
+      </c>
+      <c r="D79" s="9"/>
+      <c r="E79" s="10"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>750</v>
+      </c>
+      <c r="D80" s="9"/>
+      <c r="E80" s="10"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>1000000</v>
-      </c>
+      <c r="D81" s="9"/>
+      <c r="E81" s="10"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>1250</v>
+      </c>
+      <c r="D82" s="9"/>
+      <c r="E82" s="10"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D83" s="9"/>
+      <c r="E83" s="10"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>1750</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="10"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D85" s="9"/>
+      <c r="E85" s="10"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>2500</v>
+      </c>
+      <c r="D86" s="9"/>
+      <c r="E86" s="10"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D87" s="9"/>
+      <c r="E87" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B28:C28"/>
+  <mergeCells count="5">
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B45:C45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>